<commit_message>
fix: invalid candidate statuses in etl spreadsheet
</commit_message>
<xml_diff>
--- a/etl/dados_dw_nova.xlsx
+++ b/etl/dados_dw_nova.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Departamentos" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Usuários" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Processos" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Vagas" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Candidatos" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Vaga-Candidatos" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Entrevistas" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Feedbacks" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Contratações" sheetId="9" r:id="rId12"/>
+    <sheet name="Departamentos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Usuários" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Processos" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Vagas" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Candidatos" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Vaga-Candidatos" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Entrevistas" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Feedbacks" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Contratações" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t>dp_id</t>
   </si>
@@ -33,31 +38,31 @@
     <t>Engenharia</t>
   </si>
   <si>
-    <t>Desenvolvimento de software e hardware</t>
+    <t xml:space="preserve">Desenvolvimento de software e hardware</t>
   </si>
   <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Gestão de marca e publicidade</t>
-  </si>
-  <si>
-    <t>Recursos Humanos</t>
-  </si>
-  <si>
-    <t>Gestão de funcionários e recrutamento</t>
+    <t xml:space="preserve">Gestão de marca e publicidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos Humanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestão de funcionários e recrutamento</t>
   </si>
   <si>
     <t>Finanças</t>
   </si>
   <si>
-    <t>Planejamento financeiro e contabilidade</t>
+    <t xml:space="preserve">Planejamento financeiro e contabilidade</t>
   </si>
   <si>
     <t>Vendas</t>
   </si>
   <si>
-    <t>Desenvolvimento de negócios e relações com clientes</t>
+    <t xml:space="preserve">Desenvolvimento de negócios e relações com clientes</t>
   </si>
   <si>
     <t>usr_id</t>
@@ -78,7 +83,7 @@
     <t>usr_last_update</t>
   </si>
   <si>
-    <t>Pedro Lucas Rezende</t>
+    <t xml:space="preserve">Pedro Lucas Rezende</t>
   </si>
   <si>
     <t>pedro-l-r@example.com</t>
@@ -87,10 +92,10 @@
     <t>$pEoMmQKc1</t>
   </si>
   <si>
-    <t>Supervisor Marketing</t>
-  </si>
-  <si>
-    <t>Ana Vitória Ramos</t>
+    <t xml:space="preserve">Supervisor Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Vitória Ramos</t>
   </si>
   <si>
     <t>ana-v-r@example.com</t>
@@ -99,10 +104,10 @@
     <t>*j)@6RMbzv</t>
   </si>
   <si>
-    <t>Supervisor Engenharia</t>
-  </si>
-  <si>
-    <t>Vitor Albuquerque</t>
+    <t xml:space="preserve">Supervisor Engenharia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitor Albuquerque</t>
   </si>
   <si>
     <t>vitor-a@example.com</t>
@@ -111,10 +116,10 @@
     <t>jn+W7Zd%*6</t>
   </si>
   <si>
-    <t>Analista RH</t>
-  </si>
-  <si>
-    <t>Isabelly Novaes</t>
+    <t xml:space="preserve">Analista RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabelly Novaes</t>
   </si>
   <si>
     <t>isabelly-n@example.com</t>
@@ -123,7 +128,7 @@
     <t>_&amp;a8HpHgN*</t>
   </si>
   <si>
-    <t>Pedro Oliveira</t>
+    <t xml:space="preserve">Pedro Oliveira</t>
   </si>
   <si>
     <t>pedro-o@example.com</t>
@@ -132,10 +137,10 @@
     <t>*6^qJ1Xeek</t>
   </si>
   <si>
-    <t>Supervisor Finanças</t>
-  </si>
-  <si>
-    <t>Isaque Macedo</t>
+    <t xml:space="preserve">Supervisor Finanças</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaque Macedo</t>
   </si>
   <si>
     <t>isaque-m@example.com</t>
@@ -144,10 +149,10 @@
     <t>RRIv(ImC_7</t>
   </si>
   <si>
-    <t>Cordenador de vendas</t>
-  </si>
-  <si>
-    <t>Lavínia Sampaio</t>
+    <t xml:space="preserve">Cordenador de vendas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavínia Sampaio</t>
   </si>
   <si>
     <t>lavinia-s@example.com</t>
@@ -156,10 +161,10 @@
     <t>xn5WUEEz(2</t>
   </si>
   <si>
-    <t>Cordenador Marketing</t>
-  </si>
-  <si>
-    <t>Olívia Cassiano</t>
+    <t xml:space="preserve">Cordenador Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olívia Cassiano</t>
   </si>
   <si>
     <t>olivia-c@example.com</t>
@@ -168,10 +173,10 @@
     <t>)$3^!CZkKg</t>
   </si>
   <si>
-    <t>Gestor RH</t>
-  </si>
-  <si>
-    <t>Pietra Caldeira</t>
+    <t xml:space="preserve">Gestor RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pietra Caldeira</t>
   </si>
   <si>
     <t>pietra-c@example.com</t>
@@ -180,10 +185,10 @@
     <t>#7MH6)_^ev</t>
   </si>
   <si>
-    <t>Gestor Marketing</t>
-  </si>
-  <si>
-    <t>Mariah Moreira</t>
+    <t xml:space="preserve">Gestor Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mariah Moreira</t>
   </si>
   <si>
     <t>mariah-m@example.com</t>
@@ -192,7 +197,7 @@
     <t>xit8LMEs+f</t>
   </si>
   <si>
-    <t>Gestor Vendas</t>
+    <t xml:space="preserve">Gestor Vendas</t>
   </si>
   <si>
     <t>pc_id</t>
@@ -216,46 +221,46 @@
     <t>pc_description</t>
   </si>
   <si>
-    <t>Recrutamento Engenharia</t>
-  </si>
-  <si>
-    <t>Focado em atrair e selecionar profissionais para cargos técnicos e de desenvolvimento, como engenheiros e especialistas em tecnologia. O processo inclui avaliações técnicas e entrevistas para garantir competências específicas da área.</t>
-  </si>
-  <si>
-    <t>Recrutamento Marketing</t>
-  </si>
-  <si>
-    <t>Busca identificar talentos criativos e analíticos para posições de marketing e comunicação. As etapas podem envolver testes de portfólio, entrevistas sobre campanhas e análise de habilidades estratégicas.</t>
-  </si>
-  <si>
-    <t>Recrutamento RH</t>
-  </si>
-  <si>
-    <t>Voltado para selecionar profissionais que atuem na gestão de pessoas, incluindo especialistas em recrutamento, treinamento e desenvolvimento organizacional. O processo foca em habilidades interpessoais e conhecimento de políticas de RH.</t>
-  </si>
-  <si>
-    <t>Recrutamento Finanças</t>
-  </si>
-  <si>
-    <t>Responsável por encontrar candidatos para cargos financeiros, como analistas, contadores e tesoureiros. Envolve avaliações de raciocínio lógico e entrevistas técnicas sobre gestão financeira e conformidade regulatória.</t>
-  </si>
-  <si>
-    <t>Recrutamento Vendas</t>
-  </si>
-  <si>
-    <t>Direcionado para selecionar profissionais com habilidades de negociação e foco em resultados. O processo pode incluir simulações de vendas, entrevistas com gestores e avaliações de metas e desempenho.</t>
-  </si>
-  <si>
-    <t>Jovem Aprendiz RH</t>
-  </si>
-  <si>
-    <t>Proporcionar uma experiência de aprendizado prática no departamento de Recursos Humanos, contribuindo para o desenvolvimento profissional do jovem aprendiz e para o fortalecimento das atividades de gestão de pessoas na empresa.</t>
-  </si>
-  <si>
-    <t>Estágio em Engenharia</t>
-  </si>
-  <si>
-    <t>Oferecer uma oportunidade prática para estudantes de Engenharia, permitindo que desenvolvam habilidades técnicas e adquiram experiência no ambiente profissional, contribuindo para projetos e atividades da área.</t>
+    <t xml:space="preserve">Recrutamento Engenharia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focado em atrair e selecionar profissionais para cargos técnicos e de desenvolvimento, como engenheiros e especialistas em tecnologia. O processo inclui avaliações técnicas e entrevistas para garantir competências específicas da área.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recrutamento Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busca identificar talentos criativos e analíticos para posições de marketing e comunicação. As etapas podem envolver testes de portfólio, entrevistas sobre campanhas e análise de habilidades estratégicas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recrutamento RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltado para selecionar profissionais que atuem na gestão de pessoas, incluindo especialistas em recrutamento, treinamento e desenvolvimento organizacional. O processo foca em habilidades interpessoais e conhecimento de políticas de RH.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recrutamento Finanças</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsável por encontrar candidatos para cargos financeiros, como analistas, contadores e tesoureiros. Envolve avaliações de raciocínio lógico e entrevistas técnicas sobre gestão financeira e conformidade regulatória.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recrutamento Vendas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direcionado para selecionar profissionais com habilidades de negociação e foco em resultados. O processo pode incluir simulações de vendas, entrevistas com gestores e avaliações de metas e desempenho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jovem Aprendiz RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proporcionar uma experiência de aprendizado prática no departamento de Recursos Humanos, contribuindo para o desenvolvimento profissional do jovem aprendiz e para o fortalecimento das atividades de gestão de pessoas na empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estágio em Engenharia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oferecer uma oportunidade prática para estudantes de Engenharia, permitindo que desenvolvam habilidades técnicas e adquiram experiência no ambiente profissional, contribuindo para projetos e atividades da área.</t>
   </si>
   <si>
     <t>vc_id</t>
@@ -279,43 +284,43 @@
     <t>vc_closing_date</t>
   </si>
   <si>
-    <t>Engenheiro de Software</t>
-  </si>
-  <si>
-    <t>São Paulo</t>
-  </si>
-  <si>
-    <t>Engenheiro de Dados</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro</t>
-  </si>
-  <si>
-    <t>Analista de Marketing Digital</t>
-  </si>
-  <si>
-    <t>Minas Gerais</t>
-  </si>
-  <si>
-    <t>Especialista em SEO</t>
+    <t xml:space="preserve">Engenheiro de Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engenheiro de Dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analista de Marketing Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minas Gerais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Especialista em SEO</t>
   </si>
   <si>
     <t>Bahia</t>
   </si>
   <si>
-    <t>Analista de Recrutamento e Seleção</t>
+    <t xml:space="preserve">Analista de Recrutamento e Seleção</t>
   </si>
   <si>
     <t>Paraná</t>
   </si>
   <si>
-    <t>Especialista em Desenvolvimento Organizacional</t>
-  </si>
-  <si>
-    <t>Rio Grande do Sul</t>
-  </si>
-  <si>
-    <t>Analista Financeiro</t>
+    <t xml:space="preserve">Especialista em Desenvolvimento Organizacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analista Financeiro</t>
   </si>
   <si>
     <t>Pernambuco</t>
@@ -324,13 +329,13 @@
     <t>Tesoureiro</t>
   </si>
   <si>
-    <t>Representante de Vendas</t>
-  </si>
-  <si>
-    <t>Gerente de Vendas</t>
-  </si>
-  <si>
-    <t>Jovem Aprendiz de RH</t>
+    <t xml:space="preserve">Representante de Vendas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerente de Vendas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jovem Aprendiz de RH</t>
   </si>
   <si>
     <t>cd_id</t>
@@ -354,193 +359,193 @@
     <t>cd_last_update</t>
   </si>
   <si>
-    <t>João Lucas Porto</t>
+    <t xml:space="preserve">João Lucas Porto</t>
   </si>
   <si>
     <t>joaolucasporto@example.com</t>
   </si>
   <si>
-    <t>(11) 91234-5678</t>
-  </si>
-  <si>
-    <t>Gabriela Barros</t>
+    <t xml:space="preserve">(11) 91234-5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriela Barros</t>
   </si>
   <si>
     <t>gabrielabarros@example.com</t>
   </si>
   <si>
-    <t>(21) 98876-5432</t>
-  </si>
-  <si>
-    <t>Melissa da Rosa</t>
+    <t xml:space="preserve">(21) 98876-5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melissa da Rosa</t>
   </si>
   <si>
     <t>melissadarosa@example.com</t>
   </si>
   <si>
-    <t>(31) 99123-4567</t>
-  </si>
-  <si>
-    <t>Leandro Pereira</t>
+    <t xml:space="preserve">(31) 99123-4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leandro Pereira</t>
   </si>
   <si>
     <t>leandroperreira@example.com</t>
   </si>
   <si>
-    <t>(41) 98765-4321</t>
-  </si>
-  <si>
-    <t>Erick Câmara</t>
+    <t xml:space="preserve">(41) 98765-4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erick Câmara</t>
   </si>
   <si>
     <t>erickcamara@example.com</t>
   </si>
   <si>
-    <t>(51) 99876-5432</t>
-  </si>
-  <si>
-    <t>José Pedro Siqueira</t>
+    <t xml:space="preserve">(51) 99876-5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Pedro Siqueira</t>
   </si>
   <si>
     <t>josepedrosiqueira@example.com</t>
   </si>
   <si>
-    <t>(61) 91987-6543</t>
-  </si>
-  <si>
-    <t>Isabelly da Luz</t>
+    <t xml:space="preserve">(61) 91987-6543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabelly da Luz</t>
   </si>
   <si>
     <t>isabellydaluz@example.com</t>
   </si>
   <si>
-    <t>(71) 98765-4321</t>
-  </si>
-  <si>
-    <t>Maysa Casa Grande</t>
+    <t xml:space="preserve">(71) 98765-4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maysa Casa Grande</t>
   </si>
   <si>
     <t>maysacasagrande@example.com</t>
   </si>
   <si>
-    <t>(81) 91234-5678</t>
-  </si>
-  <si>
-    <t>Maitê Costela</t>
+    <t xml:space="preserve">(81) 91234-5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maitê Costela</t>
   </si>
   <si>
     <t>maitecostela@example.com</t>
   </si>
   <si>
-    <t>(85) 99876-5432</t>
-  </si>
-  <si>
-    <t>Isis Montenegro</t>
+    <t xml:space="preserve">(85) 99876-5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isis Montenegro</t>
   </si>
   <si>
     <t>isismontenegro@example.com</t>
   </si>
   <si>
-    <t>(91) 91923-4567</t>
-  </si>
-  <si>
-    <t>Evelyn Monteiro</t>
+    <t xml:space="preserve">(91) 91923-4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evelyn Monteiro</t>
   </si>
   <si>
     <t>evelynmonteiro@example.com</t>
   </si>
   <si>
-    <t>(98) 98876-5432</t>
-  </si>
-  <si>
-    <t>Maria Sophia Cassiano</t>
+    <t xml:space="preserve">(98) 98876-5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Sophia Cassiano</t>
   </si>
   <si>
     <t>mariasophiacassiano@example.com</t>
   </si>
   <si>
-    <t>(83) 99123-4567</t>
-  </si>
-  <si>
-    <t>Valentina Silveira</t>
+    <t xml:space="preserve">(83) 99123-4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentina Silveira</t>
   </si>
   <si>
     <t>valentinasilveira@example.com</t>
   </si>
   <si>
-    <t>(27) 98123-4567</t>
-  </si>
-  <si>
-    <t>Júlia Aragão</t>
+    <t xml:space="preserve">(27) 98123-4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Júlia Aragão</t>
   </si>
   <si>
     <t>juliaaragao@example.com</t>
   </si>
   <si>
-    <t>(22) 99999-8888</t>
-  </si>
-  <si>
-    <t>Luiz Gustavo da Cunha</t>
+    <t xml:space="preserve">(22) 99999-8888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luiz Gustavo da Cunha</t>
   </si>
   <si>
     <t>luizgustavodacunha@example.com</t>
   </si>
   <si>
-    <t>(44) 92222-3333</t>
-  </si>
-  <si>
-    <t>Maria Flor Pimenta</t>
+    <t xml:space="preserve">(44) 92222-3333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Flor Pimenta</t>
   </si>
   <si>
     <t>mariaflorpimenta@example.com</t>
   </si>
   <si>
-    <t>(15) 91234-5678</t>
-  </si>
-  <si>
-    <t>Heitor Abreu</t>
+    <t xml:space="preserve">(15) 91234-5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heitor Abreu</t>
   </si>
   <si>
     <t>heitorabreu@example.com</t>
   </si>
   <si>
-    <t>(32) 99111-2222</t>
-  </si>
-  <si>
-    <t>Natália Nogueira</t>
+    <t xml:space="preserve">(32) 99111-2222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natália Nogueira</t>
   </si>
   <si>
     <t>natalianogueira@example.com</t>
   </si>
   <si>
-    <t>(12) 99888-7777</t>
-  </si>
-  <si>
-    <t>Ian Borges</t>
+    <t xml:space="preserve">(12) 99888-7777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ian Borges</t>
   </si>
   <si>
     <t>ianborges@example.com</t>
   </si>
   <si>
-    <t>(47) 98765-4321</t>
-  </si>
-  <si>
-    <t>Maria Silva</t>
+    <t xml:space="preserve">(47) 98765-4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Silva</t>
   </si>
   <si>
     <t>maria-silva@example.com</t>
   </si>
   <si>
-    <t>(12) 98855-2233</t>
-  </si>
-  <si>
-    <t>João Borges</t>
+    <t xml:space="preserve">(12) 98855-2233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">João Borges</t>
   </si>
   <si>
     <t>joao-borges@example.com</t>
   </si>
   <si>
-    <t>(13) 96655-2244</t>
+    <t xml:space="preserve">(13) 96655-2244</t>
   </si>
   <si>
     <t>vc_cd_insert_date</t>
@@ -567,42 +572,42 @@
     <t>Aprovado</t>
   </si>
   <si>
-    <t>Harum sequi et blanditiis illo non cupiditate perspiciatis. Dolore quisquam aliquam tempora temporibus.</t>
-  </si>
-  <si>
-    <t>Minus libero itaque voluptatum. Quidem quo ipsa earum occaecati consectetur beatae.</t>
-  </si>
-  <si>
-    <t>Possimus at provident cum odio adipisci. Sequi fugit explicabo exercitationem. Explicabo numquam dolorum corrupti.
+    <t xml:space="preserve">Harum sequi et blanditiis illo non cupiditate perspiciatis. Dolore quisquam aliquam tempora temporibus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minus libero itaque voluptatum. Quidem quo ipsa earum occaecati consectetur beatae.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possimus at provident cum odio adipisci. Sequi fugit explicabo exercitationem. Explicabo numquam dolorum corrupti.
 Rem nesciunt delectus. Repellat distinctio explicabo ea minima fuga laborum dolorum.</t>
   </si>
   <si>
-    <t>Expedita molestiae illum. Corporis eligendi repudiandae reiciendis voluptas iusto corrupti. Officia occaecati omnis.</t>
-  </si>
-  <si>
-    <t>Optio earum saepe ut error. Quo ullam voluptas eaque odio. Possimus blanditiis temporibus eligendi ipsum repudiandae.
+    <t xml:space="preserve">Expedita molestiae illum. Corporis eligendi repudiandae reiciendis voluptas iusto corrupti. Officia occaecati omnis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optio earum saepe ut error. Quo ullam voluptas eaque odio. Possimus blanditiis temporibus eligendi ipsum repudiandae.
 Quo quos quibusdam similique. Non omnis eum nam maxime officiis aspernatur.</t>
   </si>
   <si>
     <t>Reprovado</t>
   </si>
   <si>
-    <t>Reprehenderit a accusantium odit numquam dicta. Architecto repellendus delectus cum.</t>
-  </si>
-  <si>
-    <t>Eligendi voluptatibus labore voluptatum alias. Dolorum aliquid ratione magnam. Magnam officiis ut velit.
+    <t xml:space="preserve">Reprehenderit a accusantium odit numquam dicta. Architecto repellendus delectus cum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eligendi voluptatibus labore voluptatum alias. Dolorum aliquid ratione magnam. Magnam officiis ut velit.
 Aspernatur dignissimos corporis officia.</t>
   </si>
   <si>
-    <t>Eos nam nobis expedita libero voluptatum.
+    <t xml:space="preserve">Eos nam nobis expedita libero voluptatum.
 Voluptate unde inventore quibusdam nemo. Aut vel deleniti mollitia ratione placeat aliquid. Quasi voluptate nam impedit.</t>
   </si>
   <si>
-    <t>Illum numquam voluptatibus quia modi. Dolor dicta harum qui rerum eius ullam. Quaerat nemo unde natus doloremque nemo assumenda recusandae.
+    <t xml:space="preserve">Illum numquam voluptatibus quia modi. Dolor dicta harum qui rerum eius ullam. Quaerat nemo unde natus doloremque nemo assumenda recusandae.
 Corporis quod repellat unde quis rerum. Cumque eos non.</t>
   </si>
   <si>
-    <t>Rerum quas molestias laboriosam eos. Illo reprehenderit quae cupiditate.</t>
+    <t xml:space="preserve">Rerum quas molestias laboriosam eos. Illo reprehenderit quae cupiditate.</t>
   </si>
   <si>
     <t>fd_id</t>
@@ -617,67 +622,67 @@
     <t>fd_content</t>
   </si>
   <si>
-    <t>Autem atque sunt ex molestias deserunt. Eum incidunt dicta itaque. Tenetur animi veniam ex doloribus quibusdam doloribus nam.</t>
-  </si>
-  <si>
-    <t>Asperiores cumque ad minus. Ipsam aliquam odio sequi explicabo quae maxime nulla. Eius ullam consequatur.</t>
-  </si>
-  <si>
-    <t>Non asperiores doloribus expedita. Mollitia voluptatibus dolores fuga.
+    <t xml:space="preserve">Autem atque sunt ex molestias deserunt. Eum incidunt dicta itaque. Tenetur animi veniam ex doloribus quibusdam doloribus nam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asperiores cumque ad minus. Ipsam aliquam odio sequi explicabo quae maxime nulla. Eius ullam consequatur.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non asperiores doloribus expedita. Mollitia voluptatibus dolores fuga.
 Sapiente corporis sint error error fugit quis fugit. Excepturi inventore quam quis.</t>
   </si>
   <si>
-    <t>Aliquam voluptates aliquid cum consequatur placeat. A quam soluta commodi ipsum.
+    <t xml:space="preserve">Aliquam voluptates aliquid cum consequatur placeat. A quam soluta commodi ipsum.
 Temporibus nostrum fugit repellendus laudantium. Exercitationem voluptas delectus at provident.</t>
   </si>
   <si>
-    <t>Eaque quod incidunt aliquam itaque veritatis molestias excepturi. Odit ad animi consectetur blanditiis sapiente. Accusantium nulla porro harum ullam similique.</t>
-  </si>
-  <si>
-    <t>Aliquid quisquam distinctio ipsa dignissimos. Cumque quisquam repellendus tempore distinctio. Distinctio tempore optio odit sit.</t>
-  </si>
-  <si>
-    <t>Ipsam saepe ullam enim architecto. Quos quas veritatis nemo quidem minus. Quidem vel quae sed unde fugiat corrupti.
+    <t xml:space="preserve">Eaque quod incidunt aliquam itaque veritatis molestias excepturi. Odit ad animi consectetur blanditiis sapiente. Accusantium nulla porro harum ullam similique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aliquid quisquam distinctio ipsa dignissimos. Cumque quisquam repellendus tempore distinctio. Distinctio tempore optio odit sit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ipsam saepe ullam enim architecto. Quos quas veritatis nemo quidem minus. Quidem vel quae sed unde fugiat corrupti.
 Qui reprehenderit non esse quos magni minima.</t>
   </si>
   <si>
-    <t>Rem voluptates blanditiis cum possimus ducimus consequatur. Doloremque voluptatem aliquam aliquid neque accusantium.</t>
-  </si>
-  <si>
-    <t>Nemo esse et excepturi. Eveniet eligendi in numquam maxime ipsum dolores. Ipsam laudantium rem occaecati veniam quaerat sed facere.</t>
-  </si>
-  <si>
-    <t>Tempore animi ratione. Ducimus laudantium soluta. Libero deserunt porro vel tenetur similique eum sapiente.
+    <t xml:space="preserve">Rem voluptates blanditiis cum possimus ducimus consequatur. Doloremque voluptatem aliquam aliquid neque accusantium.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nemo esse et excepturi. Eveniet eligendi in numquam maxime ipsum dolores. Ipsam laudantium rem occaecati veniam quaerat sed facere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempore animi ratione. Ducimus laudantium soluta. Libero deserunt porro vel tenetur similique eum sapiente.
 Voluptatem assumenda quis est. Perferendis quibusdam suscipit omnis culpa dicta.</t>
   </si>
   <si>
-    <t>Doloremque itaque culpa animi amet praesentium neque. Delectus nihil quaerat.</t>
-  </si>
-  <si>
-    <t>Vitae suscipit quasi minus odio eligendi magnam distinctio. Perferendis odio soluta cum perferendis. Culpa sint dolorem dicta quos.</t>
-  </si>
-  <si>
-    <t>Ex dolores odit sint et error provident culpa. Vero doloribus rem cum laborum qui voluptates cum.</t>
-  </si>
-  <si>
-    <t>Unde repellendus ipsam libero labore. Molestias officiis laboriosam reprehenderit hic.
+    <t xml:space="preserve">Doloremque itaque culpa animi amet praesentium neque. Delectus nihil quaerat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitae suscipit quasi minus odio eligendi magnam distinctio. Perferendis odio soluta cum perferendis. Culpa sint dolorem dicta quos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex dolores odit sint et error provident culpa. Vero doloribus rem cum laborum qui voluptates cum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unde repellendus ipsam libero labore. Molestias officiis laboriosam reprehenderit hic.
 Minus ipsum ut tempora. Repellendus optio suscipit accusantium illo voluptatibus eaque.</t>
   </si>
   <si>
-    <t>Similique tenetur reiciendis tempora earum a iste. Officiis quaerat sed est omnis esse consequuntur. Recusandae in omnis ipsam. Expedita similique dolores modi velit doloremque.</t>
-  </si>
-  <si>
-    <t>Saepe aliquam sunt. Odio fugit labore aliquid eos consequatur necessitatibus at. Debitis pariatur nihil minus eum vero. Tempora at nulla itaque.</t>
-  </si>
-  <si>
-    <t>Neque ratione eius dicta rerum. Odit repudiandae eligendi cumque inventore.
+    <t xml:space="preserve">Similique tenetur reiciendis tempora earum a iste. Officiis quaerat sed est omnis esse consequuntur. Recusandae in omnis ipsam. Expedita similique dolores modi velit doloremque.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saepe aliquam sunt. Odio fugit labore aliquid eos consequatur necessitatibus at. Debitis pariatur nihil minus eum vero. Tempora at nulla itaque.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neque ratione eius dicta rerum. Odit repudiandae eligendi cumque inventore.
 Est repudiandae vel perspiciatis. Eos quasi occaecati quaerat quidem perspiciatis molestiae.</t>
   </si>
   <si>
-    <t>Sequi distinctio accusantium. Doloribus rerum sapiente quae optio eum in. Ad eius nisi quidem culpa animi.</t>
-  </si>
-  <si>
-    <t>Doloribus fugiat qui voluptatibus. Quo voluptas soluta minus. Facilis tenetur cumque illo ut quas dignissimos. Occaecati nihil cumque doloribus quis temporibus eius.</t>
+    <t xml:space="preserve">Sequi distinctio accusantium. Doloribus rerum sapiente quae optio eum in. Ad eius nisi quidem culpa animi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doloribus fugiat qui voluptatibus. Quo voluptas soluta minus. Facilis tenetur cumque illo ut quas dignissimos. Occaecati nihil cumque doloribus quis temporibus eius.</t>
   </si>
   <si>
     <t>hr_id</t>
@@ -695,16 +700,16 @@
     <t>hr_offer_acceptance_date</t>
   </si>
   <si>
-    <t>Meio período</t>
-  </si>
-  <si>
-    <t>Tempo integral</t>
+    <t xml:space="preserve">Meio período</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo integral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
@@ -712,7 +717,7 @@
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -727,7 +732,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -737,101 +742,355 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -888,7 +1147,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -914,7 +1173,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -966,16 +1225,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -991,7 +1262,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1021,23 +1292,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.14"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="46.71"/>
-    <col customWidth="1" min="4" max="6" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="6.1399999999999997"/>
+    <col customWidth="1" min="2" max="2" width="17.289999999999999"/>
+    <col customWidth="1" min="3" max="3" width="46.710000000000001"/>
+    <col customWidth="1" min="4" max="6" width="8.7100000000000009"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1053,7 +1328,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1064,7 +1339,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1075,7 +1350,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1086,7 +1361,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -1097,7 +1372,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -2087,30 +2362,33 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.43"/>
-    <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="35.0"/>
-    <col customWidth="1" min="4" max="4" width="16.14"/>
-    <col customWidth="1" min="5" max="5" width="29.86"/>
-    <col customWidth="1" min="6" max="6" width="9.0"/>
-    <col customWidth="1" min="7" max="7" width="15.14"/>
+    <col customWidth="1" min="1" max="1" width="9.4299999999999997"/>
+    <col customWidth="1" min="2" max="2" width="22"/>
+    <col customWidth="1" min="3" max="3" width="35"/>
+    <col customWidth="1" min="4" max="4" width="34.421875"/>
+    <col customWidth="1" min="5" max="5" width="29.859999999999999"/>
+    <col customWidth="1" min="6" max="6" width="9"/>
+    <col customWidth="1" min="7" max="7" width="15.140000000000001"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2138,7 +2416,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
@@ -2153,15 +2431,15 @@
         <v>22</v>
       </c>
       <c r="F2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="3">
-        <v>45168.0</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -2176,15 +2454,15 @@
         <v>26</v>
       </c>
       <c r="F3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
-        <v>44865.0</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -2199,15 +2477,15 @@
         <v>30</v>
       </c>
       <c r="F4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3">
-        <v>45225.0</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -2222,15 +2500,15 @@
         <v>30</v>
       </c>
       <c r="F5" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>44091.0</v>
+        <v>44091</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -2245,15 +2523,15 @@
         <v>37</v>
       </c>
       <c r="F6" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G6" s="3">
-        <v>44973.0</v>
+        <v>44973</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>38</v>
@@ -2268,15 +2546,15 @@
         <v>41</v>
       </c>
       <c r="F7" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>45060.0</v>
+        <v>45060</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>42</v>
@@ -2291,15 +2569,15 @@
         <v>45</v>
       </c>
       <c r="F8" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>45128.0</v>
+        <v>45128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>46</v>
@@ -2314,15 +2592,15 @@
         <v>49</v>
       </c>
       <c r="F9" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
-        <v>45218.0</v>
+        <v>45218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
@@ -2337,15 +2615,15 @@
         <v>53</v>
       </c>
       <c r="F10" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>45460.0</v>
+        <v>45460</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>54</v>
@@ -2360,10 +2638,10 @@
         <v>57</v>
       </c>
       <c r="F11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G11" s="3">
-        <v>44458.0</v>
+        <v>44458</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>
@@ -3356,32 +3634,35 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.86"/>
+    <col customWidth="1" min="1" max="1" width="5.8600000000000003"/>
     <col customWidth="1" min="2" max="2" width="26.57"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
-    <col customWidth="1" min="4" max="4" width="22.86"/>
-    <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="6" width="9.43"/>
-    <col customWidth="1" min="7" max="7" width="6.57"/>
-    <col customWidth="1" min="8" max="8" width="129.71"/>
-    <col customWidth="1" min="9" max="9" width="6.14"/>
+    <col customWidth="1" min="3" max="3" width="14"/>
+    <col customWidth="1" min="4" max="4" width="22.859999999999999"/>
+    <col customWidth="1" min="5" max="5" width="13.859999999999999"/>
+    <col customWidth="1" min="6" max="6" width="9.4299999999999997"/>
+    <col customWidth="1" min="7" max="7" width="6.5700000000000003"/>
+    <col customWidth="1" min="8" max="8" width="129.71000000000001"/>
+    <col customWidth="1" min="9" max="9" width="6.1399999999999997"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3415,193 +3696,193 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3">
-        <v>45428.0</v>
+        <v>45428</v>
       </c>
       <c r="D2" s="3">
-        <v>45470.0</v>
+        <v>45470</v>
       </c>
       <c r="E2" s="3">
-        <v>45469.0</v>
+        <v>45469</v>
       </c>
       <c r="F2" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="I2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="3">
-        <v>45457.0</v>
+        <v>45457</v>
       </c>
       <c r="D3" s="3">
-        <v>45541.0</v>
+        <v>45541</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="I3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="3">
-        <v>45502.0</v>
+        <v>45502</v>
       </c>
       <c r="D4" s="3">
-        <v>45642.0</v>
+        <v>45642</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="I4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C5" s="3">
-        <v>45482.0</v>
+        <v>45482</v>
       </c>
       <c r="D5" s="3">
-        <v>45644.0</v>
+        <v>45644</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>72</v>
       </c>
       <c r="I5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="3">
-        <v>45278.0</v>
+        <v>45278</v>
       </c>
       <c r="D6" s="3">
-        <v>45609.0</v>
+        <v>45609</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="3">
-        <v>45516.0</v>
+        <v>45516</v>
       </c>
       <c r="D7" s="3">
-        <v>45645.0</v>
+        <v>45645</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>76</v>
       </c>
       <c r="I7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="3">
-        <v>45509.0</v>
+        <v>45509</v>
       </c>
       <c r="D8" s="3">
-        <v>45646.0</v>
+        <v>45646</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -4600,32 +4881,35 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.57"/>
-    <col customWidth="1" min="2" max="2" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.5700000000000003"/>
+    <col customWidth="1" min="2" max="2" width="8.7100000000000009"/>
     <col customWidth="1" min="3" max="3" width="21.43"/>
-    <col customWidth="1" min="4" max="4" width="19.86"/>
-    <col customWidth="1" min="5" max="5" width="12.14"/>
-    <col customWidth="1" min="6" max="6" width="18.29"/>
-    <col customWidth="1" min="7" max="7" width="9.43"/>
-    <col customWidth="1" min="8" max="8" width="18.86"/>
-    <col customWidth="1" min="9" max="9" width="17.86"/>
+    <col customWidth="1" min="4" max="4" width="19.859999999999999"/>
+    <col customWidth="1" min="5" max="5" width="12.140000000000001"/>
+    <col customWidth="1" min="6" max="6" width="18.289999999999999"/>
+    <col customWidth="1" min="7" max="7" width="9.4299999999999997"/>
+    <col customWidth="1" min="8" max="8" width="18.859999999999999"/>
+    <col customWidth="1" min="9" max="9" width="17.859999999999999"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4659,57 +4943,57 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="3">
-        <v>45435.0</v>
+        <v>45435</v>
       </c>
       <c r="I2" s="3">
-        <v>45467.0</v>
+        <v>45467</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3">
-        <v>45441.0</v>
+        <v>45441</v>
       </c>
       <c r="I3" s="3">
         <v>45533.952306666455</v>
@@ -4717,246 +5001,246 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
-        <v>45457.0</v>
+        <v>45457</v>
       </c>
       <c r="I4" s="3">
-        <v>45600.0</v>
+        <v>45600</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3">
-        <v>45457.0</v>
+        <v>45457</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D6" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="3">
-        <v>45502.0</v>
+        <v>45502</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="3">
-        <v>45502.0</v>
+        <v>45502</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G8" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>45482.0</v>
+        <v>45482</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G9" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>45482.0</v>
+        <v>45482</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D10" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G10" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H10" s="3">
-        <v>45278.0</v>
+        <v>45278</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="3">
-        <v>45285.0</v>
+        <v>45285</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="3">
-        <v>45516.0</v>
+        <v>45516</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -5977,30 +6261,33 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.86"/>
-    <col customWidth="1" min="2" max="2" width="24.29"/>
-    <col customWidth="1" min="3" max="3" width="29.29"/>
-    <col customWidth="1" min="4" max="4" width="15.14"/>
-    <col customWidth="1" min="5" max="5" width="9.43"/>
-    <col customWidth="1" min="6" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="7" width="18.86"/>
+    <col customWidth="1" min="1" max="1" width="5.8600000000000003"/>
+    <col customWidth="1" min="2" max="2" width="24.289999999999999"/>
+    <col customWidth="1" min="3" max="3" width="29.289999999999999"/>
+    <col customWidth="1" min="4" max="4" width="15.140000000000001"/>
+    <col customWidth="1" min="5" max="5" width="9.4299999999999997"/>
+    <col customWidth="1" min="6" max="6" width="8.8599999999999994"/>
+    <col customWidth="1" min="7" max="7" width="18.859999999999999"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6028,7 +6315,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>111</v>
@@ -6040,18 +6327,18 @@
         <v>113</v>
       </c>
       <c r="E2" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="G2" s="6">
-        <v>45552.89631443466</v>
+        <v>45552.896314434664</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>114</v>
@@ -6063,10 +6350,10 @@
         <v>116</v>
       </c>
       <c r="E3" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="G3" s="6">
         <v>45497.0114872376</v>
@@ -6074,7 +6361,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>117</v>
@@ -6086,10 +6373,10 @@
         <v>119</v>
       </c>
       <c r="E4" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="G4" s="6">
         <v>45533.952306666455</v>
@@ -6097,7 +6384,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>120</v>
@@ -6109,10 +6396,10 @@
         <v>122</v>
       </c>
       <c r="E5" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="G5" s="6">
         <v>45481.61523803787</v>
@@ -6120,7 +6407,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>123</v>
@@ -6132,18 +6419,18 @@
         <v>125</v>
       </c>
       <c r="E6" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="G6" s="6">
-        <v>45494.09883731219</v>
+        <v>45494.098837312187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>126</v>
@@ -6155,10 +6442,10 @@
         <v>128</v>
       </c>
       <c r="E7" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="G7" s="6">
         <v>45524.75618863252</v>
@@ -6166,7 +6453,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>129</v>
@@ -6178,10 +6465,10 @@
         <v>131</v>
       </c>
       <c r="E8" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G8" s="6">
         <v>45568.896354084914</v>
@@ -6189,7 +6476,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>132</v>
@@ -6201,18 +6488,18 @@
         <v>134</v>
       </c>
       <c r="E9" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="G9" s="6">
-        <v>45307.13833209191</v>
+        <v>45307.138332091912</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>135</v>
@@ -6224,10 +6511,10 @@
         <v>137</v>
       </c>
       <c r="E10" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="G10" s="6">
         <v>45324.062310412366</v>
@@ -6235,7 +6522,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>138</v>
@@ -6247,18 +6534,18 @@
         <v>140</v>
       </c>
       <c r="E11" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="G11" s="6">
-        <v>45345.99225260418</v>
+        <v>45345.992252604177</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>141</v>
@@ -6270,18 +6557,18 @@
         <v>143</v>
       </c>
       <c r="E12" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="G12" s="6">
-        <v>45311.61746527778</v>
+        <v>45311.617465277777</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>144</v>
@@ -6293,10 +6580,10 @@
         <v>146</v>
       </c>
       <c r="E13" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="G13" s="6">
         <v>45466.67292824074</v>
@@ -6304,7 +6591,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>147</v>
@@ -6316,18 +6603,18 @@
         <v>149</v>
       </c>
       <c r="E14" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="G14" s="6">
-        <v>45443.49652777778</v>
+        <v>45443.496527777781</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>150</v>
@@ -6339,18 +6626,18 @@
         <v>152</v>
       </c>
       <c r="E15" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="G15" s="6">
-        <v>45465.39425925926</v>
+        <v>45465.394259259258</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>153</v>
@@ -6362,18 +6649,18 @@
         <v>155</v>
       </c>
       <c r="E16" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="G16" s="6">
-        <v>45555.57803240741</v>
+        <v>45555.578032407408</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>156</v>
@@ -6385,18 +6672,18 @@
         <v>158</v>
       </c>
       <c r="E17" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="G17" s="6">
-        <v>45349.43366898148</v>
+        <v>45349.433668981481</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>159</v>
@@ -6408,10 +6695,10 @@
         <v>161</v>
       </c>
       <c r="E18" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F18" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="G18" s="6">
         <v>45322.27002314815</v>
@@ -6419,7 +6706,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>162</v>
@@ -6431,10 +6718,10 @@
         <v>164</v>
       </c>
       <c r="E19" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="G19" s="6">
         <v>45479.51767361111</v>
@@ -6442,7 +6729,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>165</v>
@@ -6454,18 +6741,18 @@
         <v>167</v>
       </c>
       <c r="E20" s="2">
-        <v>4.0</v>
+        <v>3</v>
       </c>
       <c r="F20" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="G20" s="6">
-        <v>45513.00149305556</v>
+        <v>45513.001493055563</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>168</v>
@@ -6477,18 +6764,18 @@
         <v>170</v>
       </c>
       <c r="E21" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="G21" s="6">
-        <v>45600.0</v>
+        <v>45600</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>171</v>
@@ -6500,13 +6787,13 @@
         <v>173</v>
       </c>
       <c r="E22" s="2">
-        <v>3.0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="G22" s="6">
-        <v>45600.0</v>
+        <v>45600</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -7646,26 +7933,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="8.57"/>
-    <col customWidth="1" min="3" max="3" width="19.86"/>
+    <col customWidth="1" min="1" max="1" width="8.7100000000000009"/>
+    <col customWidth="1" min="2" max="2" width="8.5700000000000003"/>
+    <col customWidth="1" min="3" max="3" width="19.859999999999999"/>
     <col customWidth="1" min="4" max="6" width="14.43"/>
   </cols>
   <sheetData>
@@ -7682,57 +7972,57 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>45538.72107638889</v>
+        <v>45538.721076388887</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6">
-        <v>45481.03247685185</v>
+        <v>45481.032476851848</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6">
-        <v>45525.78043981481</v>
+        <v>45525.780439814807</v>
       </c>
       <c r="D4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6">
-        <v>45463.84366898148</v>
+        <v>45463.843668981477</v>
       </c>
       <c r="D5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6">
         <v>45474.04519675926</v>
@@ -7741,10 +8031,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="6">
         <v>45523.47923611111</v>
@@ -7753,65 +8043,65 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C8" s="6">
-        <v>45559.92254629629</v>
+        <v>45559.922546296293</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="6">
-        <v>45298.00909722222</v>
+        <v>45298.009097222217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="6">
-        <v>45322.98016203703</v>
+        <v>45322.980162037027</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="6">
-        <v>45342.4603125</v>
+        <v>45342.460312499999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C12" s="6">
-        <v>45311.61746527778</v>
+        <v>45311.617465277777</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C13" s="6">
         <v>45466.67292824074</v>
@@ -7819,54 +8109,54 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C14" s="6">
-        <v>45443.49652777778</v>
+        <v>45443.496527777781</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6">
-        <v>45465.39425925926</v>
+        <v>45465.394259259258</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6">
-        <v>45555.57803240741</v>
+        <v>45555.578032407408</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C17" s="6">
-        <v>45349.43366898148</v>
+        <v>45349.433668981481</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6">
         <v>45322.27002314815</v>
@@ -7874,10 +8164,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C19" s="6">
         <v>45479.51767361111</v>
@@ -7885,35 +8175,35 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="6">
-        <v>45513.00149305556</v>
+        <v>45513.001493055563</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C21" s="6">
-        <v>45572.0</v>
+        <v>45572</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C22" s="6">
-        <v>45573.0</v>
+        <v>45573</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -8903,31 +9193,35 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="8.71"/>
-    <col customWidth="1" min="3" max="3" width="8.57"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="9.43"/>
-    <col customWidth="1" min="6" max="6" width="12.14"/>
-    <col customWidth="1" min="7" max="7" width="169.29"/>
-    <col customWidth="1" min="8" max="8" width="22.0"/>
-    <col customWidth="1" min="9" max="9" width="21.29"/>
+    <col customWidth="1" min="1" max="2" width="8.7100000000000009"/>
+    <col customWidth="1" min="3" max="3" width="8.5700000000000003"/>
+    <col customWidth="1" min="4" max="4" width="21.859999999999999"/>
+    <col customWidth="1" min="5" max="5" width="9.4299999999999997"/>
+    <col customWidth="1" min="6" max="6" width="12.140000000000001"/>
+    <col customWidth="1" min="7" max="7" width="169.28999999999999"/>
+    <col customWidth="1" min="8" max="8" width="22"/>
+    <col customWidth="1" min="9" max="9" width="21.289999999999999"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8961,19 +9255,19 @@
     </row>
     <row r="2">
       <c r="A2" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
         <v>45545.659931418486</v>
       </c>
       <c r="E2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>181</v>
@@ -8982,27 +9276,27 @@
         <v>182</v>
       </c>
       <c r="H2" s="3">
-        <v>45258.0</v>
+        <v>45258</v>
       </c>
       <c r="I2" s="3">
-        <v>45264.0</v>
+        <v>45264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>45486.73531275998</v>
+        <v>45486.735312759978</v>
       </c>
       <c r="E3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>181</v>
@@ -9011,27 +9305,27 @@
         <v>183</v>
       </c>
       <c r="H3" s="3">
-        <v>45454.0</v>
+        <v>45454</v>
       </c>
       <c r="I3" s="3">
-        <v>45459.0</v>
+        <v>45459</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6">
         <v>45532.0050815418</v>
       </c>
       <c r="E4" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>181</v>
@@ -9040,27 +9334,27 @@
         <v>184</v>
       </c>
       <c r="H4" s="3">
-        <v>45325.0</v>
+        <v>45325</v>
       </c>
       <c r="I4" s="3">
-        <v>45330.0</v>
+        <v>45330</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6">
-        <v>45464.91261969807</v>
+        <v>45464.912619698072</v>
       </c>
       <c r="E5" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>181</v>
@@ -9069,27 +9363,27 @@
         <v>185</v>
       </c>
       <c r="H5" s="3">
-        <v>45298.0</v>
+        <v>45298</v>
       </c>
       <c r="I5" s="3">
-        <v>45299.0</v>
+        <v>45299</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6">
-        <v>45483.36580574819</v>
+        <v>45483.365805748188</v>
       </c>
       <c r="E6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>181</v>
@@ -9098,27 +9392,27 @@
         <v>186</v>
       </c>
       <c r="H6" s="3">
-        <v>45578.0</v>
+        <v>45578</v>
       </c>
       <c r="I6" s="3">
-        <v>45582.0</v>
+        <v>45582</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6">
         <v>45524.75618863252</v>
       </c>
       <c r="E7" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>187</v>
@@ -9127,27 +9421,27 @@
         <v>188</v>
       </c>
       <c r="H7" s="3">
-        <v>45459.0</v>
+        <v>45459</v>
       </c>
       <c r="I7" s="3">
-        <v>45464.0</v>
+        <v>45464</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
         <v>45568.896354084914</v>
       </c>
       <c r="E8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>187</v>
@@ -9156,27 +9450,27 @@
         <v>189</v>
       </c>
       <c r="H8" s="3">
-        <v>45326.0</v>
+        <v>45326</v>
       </c>
       <c r="I8" s="3">
-        <v>45329.0</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="6">
-        <v>45307.13833209191</v>
+        <v>45307.138332091912</v>
       </c>
       <c r="E9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>187</v>
@@ -9185,27 +9479,27 @@
         <v>190</v>
       </c>
       <c r="H9" s="3">
-        <v>45323.0</v>
+        <v>45323</v>
       </c>
       <c r="I9" s="3">
-        <v>45331.0</v>
+        <v>45331</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D10" s="6">
         <v>45324.062310412366</v>
       </c>
       <c r="E10" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>187</v>
@@ -9214,27 +9508,27 @@
         <v>191</v>
       </c>
       <c r="H10" s="3">
-        <v>45500.0</v>
+        <v>45500</v>
       </c>
       <c r="I10" s="3">
-        <v>45501.0</v>
+        <v>45501</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D11" s="6">
-        <v>45345.99225260418</v>
+        <v>45345.992252604177</v>
       </c>
       <c r="E11" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>187</v>
@@ -9243,27 +9537,27 @@
         <v>192</v>
       </c>
       <c r="H11" s="3">
-        <v>45497.0</v>
+        <v>45497</v>
       </c>
       <c r="I11" s="3">
-        <v>45500.0</v>
+        <v>45500</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="6">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
       <c r="E12" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>181</v>
@@ -9272,27 +9566,27 @@
         <v>191</v>
       </c>
       <c r="H12" s="3">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
       <c r="I12" s="3">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="6">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
       <c r="E13" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>181</v>
@@ -9301,10 +9595,10 @@
         <v>189</v>
       </c>
       <c r="H13" s="3">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
       <c r="I13" s="3">
-        <v>45579.0</v>
+        <v>45579</v>
       </c>
     </row>
     <row r="14">
@@ -10737,30 +11031,34 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.43"/>
-    <col customWidth="1" min="2" max="2" width="8.71"/>
-    <col customWidth="1" min="3" max="3" width="8.57"/>
-    <col customWidth="1" min="4" max="4" width="48.0"/>
-    <col customWidth="1" min="5" max="5" width="10.71"/>
-    <col customWidth="1" min="6" max="6" width="153.57"/>
-    <col customWidth="1" min="7" max="7" width="9.43"/>
+    <col customWidth="1" min="1" max="1" width="8.4299999999999997"/>
+    <col customWidth="1" min="2" max="2" width="8.7100000000000009"/>
+    <col customWidth="1" min="3" max="3" width="8.5700000000000003"/>
+    <col customWidth="1" min="4" max="4" width="48"/>
+    <col customWidth="1" min="5" max="5" width="10.710000000000001"/>
+    <col customWidth="1" min="6" max="6" width="153.56999999999999"/>
+    <col customWidth="1" min="7" max="7" width="9.4299999999999997"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10788,485 +11086,485 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
         <v>45545.659931418486</v>
       </c>
       <c r="E2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>197</v>
       </c>
       <c r="G2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>45486.73531275998</v>
+        <v>45486.735312759978</v>
       </c>
       <c r="E3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>198</v>
       </c>
       <c r="G3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6">
         <v>45532.0050815418</v>
       </c>
       <c r="E4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>199</v>
       </c>
       <c r="G4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6">
-        <v>45464.91261969807</v>
+        <v>45464.912619698072</v>
       </c>
       <c r="E5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>200</v>
       </c>
       <c r="G5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6">
-        <v>45483.36580574819</v>
+        <v>45483.365805748188</v>
       </c>
       <c r="E6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>201</v>
       </c>
       <c r="G6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6">
         <v>45524.75618863252</v>
       </c>
       <c r="E7" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>202</v>
       </c>
       <c r="G7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
         <v>45568.896354084914</v>
       </c>
       <c r="E8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>203</v>
       </c>
       <c r="G8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="6">
-        <v>45307.13833209191</v>
+        <v>45307.138332091912</v>
       </c>
       <c r="E9" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>204</v>
       </c>
       <c r="G9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D10" s="6">
         <v>45324.062310412366</v>
       </c>
       <c r="E10" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>205</v>
       </c>
       <c r="G10" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D11" s="6">
-        <v>45345.99225260418</v>
+        <v>45345.992252604177</v>
       </c>
       <c r="E11" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>206</v>
       </c>
       <c r="G11" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D12" s="6">
-        <v>45311.61746527778</v>
+        <v>45311.617465277777</v>
       </c>
       <c r="E12" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>207</v>
       </c>
       <c r="G12" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D13" s="6">
         <v>45466.67292824074</v>
       </c>
       <c r="E13" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G13" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D14" s="6">
-        <v>45443.49652777778</v>
+        <v>45443.496527777781</v>
       </c>
       <c r="E14" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>209</v>
       </c>
       <c r="G14" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D15" s="6">
-        <v>45465.39425925926</v>
+        <v>45465.394259259258</v>
       </c>
       <c r="E15" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>210</v>
       </c>
       <c r="G15" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D16" s="6">
-        <v>45555.57803240741</v>
+        <v>45555.578032407408</v>
       </c>
       <c r="E16" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>211</v>
       </c>
       <c r="G16" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6">
-        <v>45349.43366898148</v>
+        <v>45349.433668981481</v>
       </c>
       <c r="E17" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G17" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="10">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D18" s="6">
         <v>45322.27002314815</v>
       </c>
       <c r="E18" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>213</v>
       </c>
       <c r="G18" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="10">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D19" s="6">
         <v>45479.51767361111</v>
       </c>
       <c r="E19" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>214</v>
       </c>
       <c r="G19" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6">
-        <v>45513.00149305556</v>
+        <v>45513.001493055563</v>
       </c>
       <c r="E20" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>215</v>
       </c>
       <c r="G20" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D21" s="6">
-        <v>45596.0</v>
+        <v>45596</v>
       </c>
       <c r="E21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>214</v>
       </c>
       <c r="G21" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D22" s="6">
-        <v>45596.0</v>
+        <v>45596</v>
       </c>
       <c r="E22" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>211</v>
       </c>
       <c r="G22" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -12644,30 +12942,33 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.71"/>
-    <col customWidth="1" min="2" max="2" width="5.86"/>
+    <col customWidth="1" min="2" max="2" width="5.8600000000000003"/>
     <col customWidth="1" min="3" max="3" width="5.71"/>
-    <col customWidth="1" min="4" max="4" width="21.14"/>
-    <col customWidth="1" min="5" max="5" width="15.14"/>
-    <col customWidth="1" min="6" max="6" width="28.14"/>
-    <col customWidth="1" min="7" max="7" width="24.0"/>
+    <col customWidth="1" min="4" max="4" width="21.140000000000001"/>
+    <col customWidth="1" min="5" max="5" width="15.140000000000001"/>
+    <col customWidth="1" min="6" max="6" width="28.140000000000001"/>
+    <col customWidth="1" min="7" max="7" width="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12695,42 +12996,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
-        <v>45549.12890505118</v>
+        <v>45549.128905051177</v>
       </c>
       <c r="E2" s="2">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>221</v>
       </c>
       <c r="G2" s="6">
-        <v>45552.89631443466</v>
+        <v>45552.896314434664</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>45487.96145064261</v>
+        <v>45487.961450642608</v>
       </c>
       <c r="E3" s="2">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>221</v>
@@ -12741,19 +13042,19 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6">
         <v>45533.768068547775</v>
       </c>
       <c r="E4" s="2">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>222</v>
@@ -12764,19 +13065,19 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6">
         <v>45474.400066998256</v>
       </c>
       <c r="E5" s="2">
-        <v>9000.0</v>
+        <v>9000</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>222</v>
@@ -12787,71 +13088,71 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6">
         <v>45487.212226968986</v>
       </c>
       <c r="E6" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>221</v>
       </c>
       <c r="G6" s="6">
-        <v>45494.09883731219</v>
+        <v>45494.098837312187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6">
-        <v>45600.0</v>
+        <v>45600</v>
       </c>
       <c r="E7" s="2">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>222</v>
       </c>
       <c r="G7" s="6">
-        <v>45594.0</v>
+        <v>45594</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
-        <v>45600.0</v>
+        <v>45600</v>
       </c>
       <c r="E8" s="2">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>222</v>
       </c>
       <c r="G8" s="6">
-        <v>45595.0</v>
+        <v>45595</v>
       </c>
     </row>
     <row r="9">
@@ -13917,9 +14218,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>